<commit_message>
Small fixes to DNR 24 data and additional summaries
</commit_message>
<xml_diff>
--- a/raw_data/wdnr/2024_LS_NS_HABs_HydroData_alldepth.xlsx
+++ b/raw_data/wdnr/2024_LS_NS_HABs_HydroData_alldepth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samblackburn/Documents/lshabs/raw_data/wdnr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFDF03D-C0FE-BB48-93E1-D1A92AA53906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEFECB1-9628-4A44-8F61-4AE285EE05E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{19CDD991-B619-4269-81A5-18F7F84FEE95}"/>
   </bookViews>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF8EB07-A391-4D8C-A9F3-0A6D0CAEB4E1}">
   <dimension ref="A1:S622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A365" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19:J23"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186:E247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6621,7 +6621,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E186" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F186">
         <v>0.5</v>
@@ -6653,7 +6653,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E187" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F187">
         <v>1</v>
@@ -6685,7 +6685,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E188" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F188">
         <v>1.5</v>
@@ -6717,7 +6717,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E189" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F189">
         <v>2</v>
@@ -6749,7 +6749,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E190" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F190">
         <v>2.5</v>
@@ -6781,7 +6781,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E191" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F191">
         <v>3</v>
@@ -6813,7 +6813,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E192" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F192">
         <v>3.5</v>
@@ -6845,7 +6845,7 @@
         <v>-91.370609999999999</v>
       </c>
       <c r="E193" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F193" s="6">
         <v>4</v>
@@ -6879,7 +6879,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E194" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F194">
         <v>0.5</v>
@@ -6911,7 +6911,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E195" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F195">
         <v>1</v>
@@ -6943,7 +6943,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E196" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F196">
         <v>1.5</v>
@@ -6975,7 +6975,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E197" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F197">
         <v>2</v>
@@ -7012,7 +7012,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E198" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F198">
         <v>2.5</v>
@@ -7049,7 +7049,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E199" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F199">
         <v>3</v>
@@ -7081,7 +7081,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E200" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F200">
         <v>3.5</v>
@@ -7113,7 +7113,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E201" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F201">
         <v>4</v>
@@ -7145,7 +7145,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E202" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F202">
         <v>4.5</v>
@@ -7177,7 +7177,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E203" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F203">
         <v>5</v>
@@ -7209,7 +7209,7 @@
         <v>-91.294280000000001</v>
       </c>
       <c r="E204" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F204" s="6">
         <v>6</v>
@@ -7243,7 +7243,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E205" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F205">
         <v>0.5</v>
@@ -7275,7 +7275,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E206" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F206">
         <v>1</v>
@@ -7307,7 +7307,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E207" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F207">
         <v>1.5</v>
@@ -7339,7 +7339,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E208" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F208">
         <v>2</v>
@@ -7371,7 +7371,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E209" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F209">
         <v>2.5</v>
@@ -7403,7 +7403,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E210" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F210">
         <v>3</v>
@@ -7435,7 +7435,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E211" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F211">
         <v>3.5</v>
@@ -7467,7 +7467,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E212" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F212">
         <v>4</v>
@@ -7499,7 +7499,7 @@
         <v>-91.264600000000002</v>
       </c>
       <c r="E213" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F213" s="6">
         <v>4.5</v>
@@ -7533,7 +7533,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E214" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F214">
         <v>0.5</v>
@@ -7565,7 +7565,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E215" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F215">
         <v>1</v>
@@ -7597,7 +7597,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E216" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F216">
         <v>1.5</v>
@@ -7629,7 +7629,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E217" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F217">
         <v>2</v>
@@ -7661,7 +7661,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E218" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F218">
         <v>2.5</v>
@@ -7693,7 +7693,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E219" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F219">
         <v>3</v>
@@ -7725,7 +7725,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E220" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F220">
         <v>3.5</v>
@@ -7757,7 +7757,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E221" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F221">
         <v>4</v>
@@ -7789,7 +7789,7 @@
         <v>-91.228059999999999</v>
       </c>
       <c r="E222" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F222" s="6">
         <v>4.5</v>
@@ -7823,7 +7823,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E223" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F223">
         <v>0.5</v>
@@ -7855,7 +7855,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E224" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F224">
         <v>1</v>
@@ -7893,7 +7893,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E225" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F225">
         <v>1.5</v>
@@ -7931,7 +7931,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E226" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F226">
         <v>2</v>
@@ -7963,7 +7963,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E227" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F227">
         <v>2.5</v>
@@ -7995,7 +7995,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E228" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F228">
         <v>3</v>
@@ -8027,7 +8027,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E229" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F229">
         <v>3.5</v>
@@ -8059,7 +8059,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E230" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F230">
         <v>4</v>
@@ -8091,7 +8091,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E231" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F231">
         <v>4.5</v>
@@ -8123,7 +8123,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E232" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F232">
         <v>5</v>
@@ -8155,7 +8155,7 @@
         <v>-91.190200000000004</v>
       </c>
       <c r="E233" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F233" s="6">
         <v>6</v>
@@ -8189,7 +8189,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E234" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F234">
         <v>0.5</v>
@@ -8221,7 +8221,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E235" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F235">
         <v>1</v>
@@ -8253,7 +8253,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E236" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F236">
         <v>1.5</v>
@@ -8285,7 +8285,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E237" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F237">
         <v>2</v>
@@ -8317,7 +8317,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E238" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F238">
         <v>2.5</v>
@@ -8349,7 +8349,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E239" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F239">
         <v>3</v>
@@ -8381,7 +8381,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E240" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F240">
         <v>3.5</v>
@@ -8413,7 +8413,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E241" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F241">
         <v>4</v>
@@ -8445,7 +8445,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E242" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F242">
         <v>4.5</v>
@@ -8477,7 +8477,7 @@
         <v>-91.115295000000003</v>
       </c>
       <c r="E243" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F243" s="6">
         <v>5</v>
@@ -8511,7 +8511,7 @@
         <v>-91.061499999999995</v>
       </c>
       <c r="E244" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F244">
         <v>0.5</v>
@@ -8543,7 +8543,7 @@
         <v>-91.061499999999995</v>
       </c>
       <c r="E245" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F245">
         <v>1</v>
@@ -8575,7 +8575,7 @@
         <v>-91.061499999999995</v>
       </c>
       <c r="E246" s="4">
-        <v>45484</v>
+        <v>45482</v>
       </c>
       <c r="F246">
         <v>1.5</v>
@@ -8606,8 +8606,8 @@
       <c r="D247" s="17">
         <v>-91.061499999999995</v>
       </c>
-      <c r="E247" s="18">
-        <v>45484</v>
+      <c r="E247" s="4">
+        <v>45482</v>
       </c>
       <c r="F247" s="17">
         <v>2</v>
@@ -21251,80 +21251,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Draft</_Status>
-    <Contract_x0020_Organization xmlns="ce7dfae9-3368-4e15-961b-dfb270657697" xsi:nil="true"/>
-    <AOC xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">
-      <Value>Undefined</Value>
-    </AOC>
-    <Document_x0020_Category xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">15</Document_x0020_Category>
-    <Grant_x0020_Name_x0020_and_x0020_Number xmlns="f5104109-d43e-4c14-a52e-7e70ffd3d049">41</Grant_x0020_Name_x0020_and_x0020_Number>
-    <Project_x0020_Name_x0020_and_x0020_Number xmlns="f5104109-d43e-4c14-a52e-7e70ffd3d049">166</Project_x0020_Name_x0020_and_x0020_Number>
-    <_dlc_DocId xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b">WDNREMSP-2100715649-1815</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b">
-      <Url>https://wigov.sharepoint.com/sites/dnr-tem/Office-GW/_layouts/15/DocIdRedir.aspx?ID=WDNREMSP-2100715649-1815</Url>
-      <Description>WDNREMSP-2100715649-1815</Description>
-    </_dlc_DocIdUrl>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023C77F7B5D1C27459F2E5BA5E7361F04" ma:contentTypeVersion="30" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27cdd19e9f7b5e3d886be36b407a81c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0a621863-9757-48d1-a1a6-8e3cccba451b" xmlns:ns3="f5104109-d43e-4c14-a52e-7e70ffd3d049" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="ce7dfae9-3368-4e15-961b-dfb270657697" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64e5fec3e76bedfb2da1959a4e034eec" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="0a621863-9757-48d1-a1a6-8e3cccba451b"/>
@@ -21641,37 +21576,89 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Draft</_Status>
+    <Contract_x0020_Organization xmlns="ce7dfae9-3368-4e15-961b-dfb270657697" xsi:nil="true"/>
+    <AOC xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">
+      <Value>Undefined</Value>
+    </AOC>
+    <Document_x0020_Category xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">15</Document_x0020_Category>
+    <Grant_x0020_Name_x0020_and_x0020_Number xmlns="f5104109-d43e-4c14-a52e-7e70ffd3d049">41</Grant_x0020_Name_x0020_and_x0020_Number>
+    <Project_x0020_Name_x0020_and_x0020_Number xmlns="f5104109-d43e-4c14-a52e-7e70ffd3d049">166</Project_x0020_Name_x0020_and_x0020_Number>
+    <_dlc_DocId xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b">WDNREMSP-2100715649-1815</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b">
+      <Url>https://wigov.sharepoint.com/sites/dnr-tem/Office-GW/_layouts/15/DocIdRedir.aspx?ID=WDNREMSP-2100715649-1815</Url>
+      <Description>WDNREMSP-2100715649-1815</Description>
+    </_dlc_DocIdUrl>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce7dfae9-3368-4e15-961b-dfb270657697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0a621863-9757-48d1-a1a6-8e3cccba451b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D70670EE-0991-4E0E-B7E0-9987BBEB934D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{445EA51C-6E17-49DA-AC40-943EA434FA27}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="ce7dfae9-3368-4e15-961b-dfb270657697"/>
-    <ds:schemaRef ds:uri="f5104109-d43e-4c14-a52e-7e70ffd3d049"/>
-    <ds:schemaRef ds:uri="0a621863-9757-48d1-a1a6-8e3cccba451b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3928F6FF-9520-471F-9EB0-C0799DBFBDB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AD60D9D-65A4-4E12-A02B-E31CF0654367}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21692,10 +21679,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3928F6FF-9520-471F-9EB0-C0799DBFBDB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{445EA51C-6E17-49DA-AC40-943EA434FA27}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D70670EE-0991-4E0E-B7E0-9987BBEB934D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="ce7dfae9-3368-4e15-961b-dfb270657697"/>
+    <ds:schemaRef ds:uri="f5104109-d43e-4c14-a52e-7e70ffd3d049"/>
+    <ds:schemaRef ds:uri="0a621863-9757-48d1-a1a6-8e3cccba451b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>